<commit_message>
best I can do with the figures
</commit_message>
<xml_diff>
--- a/Poster/graphics work.xlsx
+++ b/Poster/graphics work.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="9555" windowHeight="8385" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="9555" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart4" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <sheet name="Sheet7" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -861,11 +860,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="43630592"/>
-        <c:axId val="77561856"/>
+        <c:axId val="65011200"/>
+        <c:axId val="79813376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43630592"/>
+        <c:axId val="65011200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,7 +893,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77561856"/>
+        <c:crossAx val="79813376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -902,7 +901,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77561856"/>
+        <c:axId val="79813376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -932,7 +931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43630592"/>
+        <c:crossAx val="65011200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6270,11 +6269,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="77563584"/>
-        <c:axId val="77564160"/>
+        <c:axId val="67527232"/>
+        <c:axId val="67527808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77563584"/>
+        <c:axId val="67527232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="450"/>
@@ -6288,10 +6287,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>Representative Number</a:t>
                 </a:r>
               </a:p>
@@ -6304,12 +6303,22 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77564160"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67527808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77564160"/>
+        <c:axId val="67527808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -6325,10 +6334,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>Percent Accuracy</a:t>
                 </a:r>
               </a:p>
@@ -6341,7 +6350,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77563584"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67527232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6350,6 +6369,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -6555,7 +6584,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6904,11 +6932,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40441856"/>
-        <c:axId val="45695552"/>
+        <c:axId val="64985600"/>
+        <c:axId val="67531264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40441856"/>
+        <c:axId val="64985600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6930,14 +6958,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45695552"/>
+        <c:crossAx val="67531264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6945,7 +6972,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45695552"/>
+        <c:axId val="67531264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6968,21 +6995,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40441856"/>
+        <c:crossAx val="64985600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12320,11 +12345,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45697856"/>
-        <c:axId val="45698432"/>
+        <c:axId val="67533568"/>
+        <c:axId val="67534144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45697856"/>
+        <c:axId val="67533568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12334,12 +12359,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45698432"/>
+        <c:crossAx val="67534144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45698432"/>
+        <c:axId val="67534144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -12352,14 +12377,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45697856"/>
+        <c:crossAx val="67533568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12399,7 +12423,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -12535,11 +12558,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="167864320"/>
-        <c:axId val="47383680"/>
+        <c:axId val="67972608"/>
+        <c:axId val="127076032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="167864320"/>
+        <c:axId val="67972608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12561,7 +12584,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -12577,7 +12599,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47383680"/>
+        <c:crossAx val="127076032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12585,7 +12607,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47383680"/>
+        <c:axId val="127076032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12608,7 +12630,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -12625,7 +12646,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167864320"/>
+        <c:crossAx val="67972608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17988,11 +18009,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="105855744"/>
-        <c:axId val="163074560"/>
+        <c:axId val="127077760"/>
+        <c:axId val="127078336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105855744"/>
+        <c:axId val="127077760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3500"/>
@@ -18015,7 +18036,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -18032,12 +18052,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="163074560"/>
+        <c:crossAx val="127078336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="163074560"/>
+        <c:axId val="127078336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -18067,7 +18087,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -18084,14 +18103,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105855744"/>
+        <c:crossAx val="127077760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -18155,7 +18173,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="131" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18210,7 +18228,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="131" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>